<commit_message>
English version is completely
Please check it again and tell me or edit it if anything wrong.
</commit_message>
<xml_diff>
--- a/thailand_earthquake_stat 2547-2557_eng_version.xlsx
+++ b/thailand_earthquake_stat 2547-2557_eng_version.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="531">
   <si>
     <t>DATE</t>
   </si>
@@ -46,9 +46,6 @@
     <t>1.9 Ml</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนที่ อ.สันทราย อ.ดอยสะเก็ด จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t>27 มี.ค. 47</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>3.7Ml</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.เมือง อ.หางดง จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t>17 ก.ย. 47</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>5.8 Ml</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้บนอาคารสูงของ กทม.</t>
-  </si>
-  <si>
     <t>26 ธ.ค. 47</t>
   </si>
   <si>
@@ -127,18 +118,12 @@
     <t>8.0Ml</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้เกือบทุกจังหวัดในภาคใต้ รวมถึงอาคารสูงหลายแห่งใน กทม.และเกิดคลื่นสึนามิก่อให้เกิดความเสียหายอย่างมากบริเวณภาคใต้ ฝั่งตะวันตก มีผู้เสียชีวิตกว่า 5,000 คน</t>
-  </si>
-  <si>
     <t>20.7N 98.0E</t>
   </si>
   <si>
     <t>6.4Ml</t>
   </si>
   <si>
-    <t>รู้สึกได้หลายจังหวัดในภาคเหนือ ได้แก่ ลำปาง เชียงใหม่ เชียงราย และกทม.</t>
-  </si>
-  <si>
     <t>27 ธ.ค. 47</t>
   </si>
   <si>
@@ -151,9 +136,6 @@
     <t>6.6Ml</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่จังหวัดภูเก็ต</t>
-  </si>
-  <si>
     <t>30 ธ.ค. 47</t>
   </si>
   <si>
@@ -163,9 +145,6 @@
     <t>5.4,5.6Ml</t>
   </si>
   <si>
-    <t>รู้สึกได้บนอาคารสูงใน อ.เมือง จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t>9 ก.พ. 2548</t>
   </si>
   <si>
@@ -175,9 +154,6 @@
     <t xml:space="preserve">5.8 </t>
   </si>
   <si>
-    <t>รู้สึกได้ที่ อ.เมือง จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t>16 ก.พ. 2548</t>
   </si>
   <si>
@@ -190,9 +166,6 @@
     <t>5.8</t>
   </si>
   <si>
-    <t>รู้สึกได้บนอาคารสูง จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t>28 มี.ค. 2548</t>
   </si>
   <si>
@@ -205,9 +178,6 @@
     <t>8.5</t>
   </si>
   <si>
-    <t>ห่างจาก จ.ภูเก็ต ไปทางทิศตะวันตกเฉียงใต้ ประมาณ 670 กม.มีคำเตือนให้ประชาชนอพยพ</t>
-  </si>
-  <si>
     <t xml:space="preserve">10 เม.ย.2548 </t>
   </si>
   <si>
@@ -220,9 +190,6 @@
     <t xml:space="preserve">6.7 </t>
   </si>
   <si>
-    <t xml:space="preserve"> ไม่มีรายงานความสั่นสะเทือนในประเทศไทย</t>
-  </si>
-  <si>
     <t xml:space="preserve">14 พ.ค. 2548 </t>
   </si>
   <si>
@@ -247,9 +214,6 @@
     <t>6.8</t>
   </si>
   <si>
-    <t>รู้สึกได้หลายจังหวัดในภาคใต้ตอนล่าง และบนอาคารสูงบางแห่งในกรุงเทพฯ</t>
-  </si>
-  <si>
     <t xml:space="preserve">22 พ.ค. 2548 </t>
   </si>
   <si>
@@ -262,9 +226,6 @@
     <t>6.1</t>
   </si>
   <si>
-    <t>ไม่มีรายงานความสั่นสะเทือนในประเทศไทย</t>
-  </si>
-  <si>
     <t>5 มิ.ย. 2548</t>
   </si>
   <si>
@@ -277,9 +238,6 @@
     <t>2.8</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้เล็กน้อยในบริเวณใกล้ศูนย์กลาง</t>
-  </si>
-  <si>
     <t>08.53 น.</t>
   </si>
   <si>
@@ -289,9 +247,6 @@
     <t>3.0</t>
   </si>
   <si>
-    <t>ห่างจาก จ.เชียงใหม่ ไปทางทิศใต้ประมาณ 110 กม.</t>
-  </si>
-  <si>
     <t xml:space="preserve">5 ก.ค. 2548 </t>
   </si>
   <si>
@@ -304,9 +259,6 @@
     <t xml:space="preserve">6.8 </t>
   </si>
   <si>
-    <t>ห่างจาก จ.ภูเก็ตไปทางทิศตะวันตกเฉียงใต้ประมาณ 700 กม.</t>
-  </si>
-  <si>
     <t>24 ก.ค. 2548</t>
   </si>
   <si>
@@ -319,9 +271,6 @@
     <t>7.2</t>
   </si>
   <si>
-    <t>ห่างจาก จ.ภูเก็ตไปทางทิศตะวันตกเฉียงใต้ ประมาณ 640 กม. เตือนให้ประชาชนอพยพ</t>
-  </si>
-  <si>
     <t>7 ก.ย. 2548</t>
   </si>
   <si>
@@ -334,9 +283,6 @@
     <t>5.0</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ จ.พังงาและ จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t xml:space="preserve">18 ก.ย. 2548 </t>
   </si>
   <si>
@@ -349,9 +295,6 @@
     <t xml:space="preserve">6.0 </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนบนอาคารสูง จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t>11 ต.ค.2548</t>
   </si>
   <si>
@@ -373,36 +316,24 @@
     <t xml:space="preserve">2.20 N 96.50E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ จ.พังงา และ จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t>4 ธ.ค. 2548</t>
   </si>
   <si>
     <t>16.34 น.</t>
   </si>
   <si>
-    <t xml:space="preserve">จ.เชียงใหม่ </t>
-  </si>
-  <si>
     <t xml:space="preserve">18.70 N 98.50 E </t>
   </si>
   <si>
     <t>4.1</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้บนอาคารสูง จ.เชียงใหม่ และ จ.ลำพูน </t>
-  </si>
-  <si>
     <t>7 ธ.ค. 2548</t>
   </si>
   <si>
     <t>16.02 น.</t>
   </si>
   <si>
-    <t xml:space="preserve">จ.เชียงราย </t>
-  </si>
-  <si>
     <t>19.70N 99.60E</t>
   </si>
   <si>
@@ -418,9 +349,6 @@
     <t xml:space="preserve">19.43N 100.18E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.เมือง อ.เทิง จ.เชียงราย</t>
-  </si>
-  <si>
     <t>16 ธ.ค. 2548</t>
   </si>
   <si>
@@ -433,9 +361,6 @@
     <t>3.8, 3.9</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.ป่าแดด จ.เชียงราย</t>
-  </si>
-  <si>
     <t>24 ม.ค. 2549</t>
   </si>
   <si>
@@ -448,18 +373,12 @@
     <t xml:space="preserve">5.7 </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ จ.เชียงใหม่ เชียงราย แม่ฮ่องสอน</t>
-  </si>
-  <si>
     <t>16 มี.ค.2549</t>
   </si>
   <si>
     <t>20.34 น.</t>
   </si>
   <si>
-    <t>เชียงใหม่</t>
-  </si>
-  <si>
     <t xml:space="preserve">3.0 </t>
   </si>
   <si>
@@ -472,9 +391,6 @@
     <t xml:space="preserve">18.8 N 98.8 E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.หางดง อ.สันป่าตอง จ. เชียงใหม่</t>
-  </si>
-  <si>
     <t>6 ส.ค.2549</t>
   </si>
   <si>
@@ -487,9 +403,6 @@
     <t>3.4</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.เชียงดาว จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t xml:space="preserve">27 ก.ย.2549 </t>
   </si>
   <si>
@@ -502,9 +415,6 @@
     <t>4.8</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้เกือบทั่วไปของจังหวัดประจวบคีรีขันธ์ </t>
-  </si>
-  <si>
     <t xml:space="preserve">28 ก.ย.2549 </t>
   </si>
   <si>
@@ -538,9 +448,6 @@
     <t>5.6</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้เกือบทั่วไปของจังหวัดประจวบคีรีขันธ์ ,อ.ท่ายาง จ.เพชรบุรี อ.โพธาราม จ.ราชบุรี,อ.เมือง จ.สมุทรสงคราม</t>
-  </si>
-  <si>
     <t>17 พ.ย 2549</t>
   </si>
   <si>
@@ -562,9 +469,6 @@
     <t xml:space="preserve">3.49 N 99.2 E </t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้ที่ อ.หาดใหญ่ จ.สงขลา และ จ.นราธิวาส </t>
-  </si>
-  <si>
     <t xml:space="preserve">13 ธ.ค. 2549 </t>
   </si>
   <si>
@@ -577,9 +481,6 @@
     <t>5.1</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้เกือบทั่วไปใน จ.เชียงใหม่ และอาคารสูงใน จ.เชียงราย</t>
-  </si>
-  <si>
     <t>19 ธ.ค. 2549</t>
   </si>
   <si>
@@ -613,9 +514,6 @@
     <t xml:space="preserve">3.3 </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่บริเวณ จ.แม่ฮ่องสอน</t>
-  </si>
-  <si>
     <t>23 ธ.ค. 2549</t>
   </si>
   <si>
@@ -661,9 +559,6 @@
     <t xml:space="preserve"> 6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้ที่ จ.ภูเก็ต </t>
-  </si>
-  <si>
     <t>15 พ.ค. 2550</t>
   </si>
   <si>
@@ -673,9 +568,6 @@
     <t xml:space="preserve"> 20.87 N 100.74 E</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ จ.เชียงราย</t>
-  </si>
-  <si>
     <t>16 พ.ค. 2550</t>
   </si>
   <si>
@@ -685,9 +577,6 @@
     <t>21.1 N 100.32 E</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้ที่ หลายจังหวัดในภาคเหนือและอาคารสูงในกรุงเทพมหานคร </t>
-  </si>
-  <si>
     <t>19 มิ.ย. 2550</t>
   </si>
   <si>
@@ -706,18 +595,12 @@
     <t xml:space="preserve">15.17,15.27 น. </t>
   </si>
   <si>
-    <t xml:space="preserve">พม่า </t>
-  </si>
-  <si>
     <t xml:space="preserve">21.27 N 99.82 E </t>
   </si>
   <si>
     <t>5.5,5.2</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.เชียงแสน จ.เชียงราย และอาคารสูงในกรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>12 ก.ย. 2550</t>
   </si>
   <si>
@@ -730,9 +613,6 @@
     <t>8.4</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้บนอาคารสูง ในกรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>13 ก.ย. 2550</t>
   </si>
   <si>
@@ -745,9 +625,6 @@
     <t>7.1</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ บนอาคารสูงบางแห่ง ในกรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>16 ต.ค. 2550</t>
   </si>
   <si>
@@ -778,9 +655,6 @@
     <t>5.42 N 95.91E</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้บนอาคารสูง จ.ภูเก็ต จ.พังงา </t>
-  </si>
-  <si>
     <t>20 ก.พ.51</t>
   </si>
   <si>
@@ -793,9 +667,6 @@
     <t>7.5</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบนตึกสูงในกรุงเทพฯและจ.ภูเก็ต อาจเกิดสึนามิขนาดเล็กบริเวณใกล้ศูนย์กลาง</t>
-  </si>
-  <si>
     <t>22 เม.ย.51</t>
   </si>
   <si>
@@ -817,9 +688,6 @@
     <t>7.8</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบนตึกสูงในกรุงเทพฯหลายแห่ง ประเทศจีนมีผู้เสียชีวิตประมาณ 20,000 คน</t>
-  </si>
-  <si>
     <t>1 ก.ค.51</t>
   </si>
   <si>
@@ -832,9 +700,6 @@
     <t>3.8</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวได้ที่ จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t>21 สิงหาคม 2551</t>
   </si>
   <si>
@@ -844,9 +709,6 @@
     <t xml:space="preserve">25.1 N 97.82 E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบนตึกสูงในกรุงเทพฯหลายแห่ง ประเทศจีนมีผู้เสียชีวิต 1 คน บาดเจ็บหลายคน</t>
-  </si>
-  <si>
     <t>22 กันยายน 51</t>
   </si>
   <si>
@@ -859,9 +721,6 @@
     <t>5.2</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบนตึกสูงหลายแห่งในกรุงเทพ</t>
-  </si>
-  <si>
     <t>23 ธันวาคม 2551</t>
   </si>
   <si>
@@ -883,9 +742,6 @@
     <t>7.9</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นไหวบนตึกสูงในกรุงเทพฯ ประเทศอินโดนีเซียมีผู้เสียชีวิตประมาณ 1000 คน </t>
-  </si>
-  <si>
     <t xml:space="preserve">20 มีนาคม 2553 </t>
   </si>
   <si>
@@ -922,9 +778,6 @@
     <t>7.6</t>
   </si>
   <si>
-    <t>รู้สึกได้ที่อาคารสูงกทม. หลายแห่ง</t>
-  </si>
-  <si>
     <t>9 พฤษภาคม 2553</t>
   </si>
   <si>
@@ -937,9 +790,6 @@
     <t>7.3</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวอาคารสูง จ. ภูเก็ต พังงา สุราษฏร์ธานี จ. สงขลาและ กรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>6 กรกฎาคม 2553</t>
   </si>
   <si>
@@ -949,9 +799,6 @@
     <t xml:space="preserve">20.42 N 99.83 E </t>
   </si>
   <si>
-    <t>รู้สึกได้ที่ อ.แม่สาย อ.แม่จัน อ. เชียงแสน อ.แม่ฟ้าหลวง จ.เชียงราย</t>
-  </si>
-  <si>
     <t>4 กุมภาพันธ์ 2554</t>
   </si>
   <si>
@@ -961,27 +808,18 @@
     <t>24.64 N 99.73 E</t>
   </si>
   <si>
-    <t>รู้สึกบนอาคารสูง กทม. หลายแห่ง</t>
-  </si>
-  <si>
     <t>23 กุมภาพันธ์ 2554</t>
   </si>
   <si>
     <t>22:53</t>
   </si>
   <si>
-    <t xml:space="preserve">ลาว </t>
-  </si>
-  <si>
     <t>18.82N 101.74 E</t>
   </si>
   <si>
     <t>5.4</t>
   </si>
   <si>
-    <t>รู้สึกที่ แพร่ น่าน อุดรธานี เลย หนองคาย หนองบัวลำภู ขอนแก่น มหาสารคาม</t>
-  </si>
-  <si>
     <t>24 มีนาคม 2554</t>
   </si>
   <si>
@@ -994,9 +832,6 @@
     <t>6.7</t>
   </si>
   <si>
-    <t>รู้สึกได้ในภาคเหนือ ตะวันออกเฉียงเหนือและ อาคาร สูงในกทม.หลายแห่ง และมีความเสียหายที่ อ.แม่สาย จ.เชียงราย มีผู้เสียชีวิต 1 คนจากผนังบ้านพังทับศรีษะ</t>
-  </si>
-  <si>
     <t>30 เมษายน 2554</t>
   </si>
   <si>
@@ -1006,9 +841,6 @@
     <t>7.39 N 97.76 E</t>
   </si>
   <si>
-    <t>รู้สึกที่ จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t>10 พฤษภาคม 2554</t>
   </si>
   <si>
@@ -1021,9 +853,6 @@
     <t>4.0</t>
   </si>
   <si>
-    <t>รู้สึกที่ อ.แม่สาย จ.เชียงราย</t>
-  </si>
-  <si>
     <t>24 มิถุนายน 2554</t>
   </si>
   <si>
@@ -1033,9 +862,6 @@
     <t>7.38 N 99.63 E</t>
   </si>
   <si>
-    <t>รู้สึกที่ อ.กันตัง อ.ย่านตาขาว อ.เมือง จ.ตรัง</t>
-  </si>
-  <si>
     <t>6 กันยายน 2554</t>
   </si>
   <si>
@@ -1045,9 +871,6 @@
     <t>2.79 N 97.7 E</t>
   </si>
   <si>
-    <t>รู้สึกที่ อ.เมือง จ.ภูเก็ต อ.หาดใหญ่ จ.สงขลา</t>
-  </si>
-  <si>
     <t>20 กุมภาพันธ์ 2555</t>
   </si>
   <si>
@@ -1060,9 +883,6 @@
     <t xml:space="preserve">2.7 </t>
   </si>
   <si>
-    <t>รู้สึกได้บริเวณใกล้ศูนย์กลาง และมีความเสียหายเล็กน้อย</t>
-  </si>
-  <si>
     <t>5 มีนาคม 2555</t>
   </si>
   <si>
@@ -1072,9 +892,6 @@
     <t>4.15 N 97.11 E</t>
   </si>
   <si>
-    <t>รู้สึกไหวเล็กน้อยที่ จ. ภูเก็ต</t>
-  </si>
-  <si>
     <t>11 เมษายน 2555</t>
   </si>
   <si>
@@ -1087,9 +904,6 @@
     <t>8.6</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกได้ในหลายจังหวัดในภาคใต้และภาคกลาง รวมถึง ภาคอีสาน เกิดคลื่นสึนามิสูง 80ซม.ที่ประเทศอินโดนีเซีย และ30ซม. ที่เกาะเมียง จ.พังงา </t>
-  </si>
-  <si>
     <t>16 เมษายน 2555</t>
   </si>
   <si>
@@ -1102,9 +916,6 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>รู้สึกไหวในหลายพื้นที่ใน จ. ภูเก็ต บ้านเรือนแตกร้าวหลายหลัง ในอ.ถลาง จ. ภูเก็ต เกิดอัฟเตอร์ช็อคมากกว่า 26 ครั้ง</t>
-  </si>
-  <si>
     <t>4 มิถุนายน 2555</t>
   </si>
   <si>
@@ -1114,9 +925,6 @@
     <t>9.84N 98.58E</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ ต.เขานิเวศน์ ต.บางนอน อ.เมืองระนอง จ.ระนอง</t>
-  </si>
-  <si>
     <t>23 มิถุนายน 2555</t>
   </si>
   <si>
@@ -1129,9 +937,6 @@
     <t>6.3</t>
   </si>
   <si>
-    <t>รู้สึกบนอาคารสูง จ.ภูเก็ตและ สงขลา</t>
-  </si>
-  <si>
     <t>13 กันยายน 2555</t>
   </si>
   <si>
@@ -1153,18 +958,12 @@
     <t>6.6</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ จ.เชียงใหม่ จ.นนทบุรี จ.กรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>17:54</t>
   </si>
   <si>
     <t xml:space="preserve">22.74N,95.93E  </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ จ.เชียงใหม่ และบนตึกสูงของ จ.กรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>20 ธันวาคม 2555</t>
   </si>
   <si>
@@ -1177,9 +976,6 @@
     <t>4.6</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่อำเภอแม่สาย จังหวัดเชียงราย และบนอาคารสูงจังหวัดเชียงใหม่</t>
-  </si>
-  <si>
     <t>7 กุมภาพันธ์ 2556</t>
   </si>
   <si>
@@ -1189,9 +985,6 @@
     <t xml:space="preserve">21.10N,99.85E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ อ.แม่สาย จ.เชียงราย</t>
-  </si>
-  <si>
     <t>2 มีนาคม 2556</t>
   </si>
   <si>
@@ -1201,9 +994,6 @@
     <t xml:space="preserve">18.36N,99.56E </t>
   </si>
   <si>
-    <t xml:space="preserve">ได้ยินเสียงดัง บ้านมีการสั่น รู้สึกสั่นไหวที่ ต.ต้นฝาย ต.พิชัย ต.ต้นธงชัย จ.ลำปาง </t>
-  </si>
-  <si>
     <t>5 เมษายน 2556</t>
   </si>
   <si>
@@ -1216,9 +1006,6 @@
     <t>2.9</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นไหวที่ อ.แม่วาง อ.หางดง อ.เมือง จ.เชียงใหม่ </t>
-  </si>
-  <si>
     <t>11 เมษายน 2556</t>
   </si>
   <si>
@@ -1228,9 +1015,6 @@
     <t xml:space="preserve">18.96N,97.68E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ จ.แม่ฮ่องสอน</t>
-  </si>
-  <si>
     <t>7 พฤษภาคม 2556</t>
   </si>
   <si>
@@ -1249,9 +1033,6 @@
     <t xml:space="preserve">18.61N,98.74E  </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ อ.แม่วาง อ.สันป่าตอง จ.เชียงใหม่</t>
-  </si>
-  <si>
     <t>2 กรกฎาคม 2556</t>
   </si>
   <si>
@@ -1264,9 +1045,6 @@
     <t>6.0</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบริเวณ จ.ภูเก็ต จ.พังงา และอาคารสูงในกรุงเทพฯ</t>
-  </si>
-  <si>
     <t>1 สิงหาคม 2556</t>
   </si>
   <si>
@@ -1279,9 +1057,6 @@
     <t>3.7</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ อ.แม่ใจ จ.พะเยา</t>
-  </si>
-  <si>
     <t>20 กันยายน 2556</t>
   </si>
   <si>
@@ -1327,9 +1102,6 @@
     <t>6.4</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ อ.เมือง จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t>5 พฤษภาคม 2557</t>
   </si>
   <si>
@@ -1339,18 +1111,12 @@
     <t>19.75N, 99.69E</t>
   </si>
   <si>
-    <t>ถนน อาคารและบ้านเรือน บริเวณใกล้จุดศูนย์กลางได้รับความเสียหายอย่างหนัก มีผู้เสียชีวิต 1 คน เกิดโคลนผุด รู้สึกสั่นไหวที่ จ.เชียงราย, จ.แพร่, จ.แม่ฮ่องสอน, จ.อุตรดิตถ์, จ.พิษณุโลก, จ.เชียงใหม่และตึกสูงในกรุงเทพมหานครฯ</t>
-  </si>
-  <si>
     <t>24 พฤษภาคม 2557</t>
   </si>
   <si>
     <t>18.40N, 100.77E</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ ต.ในเวียง อ.เมือง จ.น่าน</t>
-  </si>
-  <si>
     <t>24 ตุลาคม 2557</t>
   </si>
   <si>
@@ -1375,9 +1141,6 @@
     <t>5.9</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ ตึกสูง จ.เชียงราย, จ.เชียงใหม่และกรุงเทพมหานคร</t>
-  </si>
-  <si>
     <t>19 มกราคม 2558</t>
   </si>
   <si>
@@ -1393,24 +1156,15 @@
     <t>13:02</t>
   </si>
   <si>
-    <t>อ่าวพังงา ทางทิศใต้ของเกาะยาวใหญ่ อ.เกาะยาว จ.พังงา</t>
-  </si>
-  <si>
     <t>7.87N, 98.57E</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ อ.เมือง อ.กะทู้ อ.ถลาง จ.ภูเก็ต, เกาะยาวใหญ่ จ.พังงา</t>
-  </si>
-  <si>
     <t>25 มีนาคม 2558</t>
   </si>
   <si>
     <t>05:32</t>
   </si>
   <si>
-    <t>นอกชายฝั่งทางทิศตะวันออกของ จ.ภูเก็ต</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.89N, 98.52E </t>
   </si>
   <si>
@@ -1420,30 +1174,18 @@
     <t>04:18</t>
   </si>
   <si>
-    <t>ในทะเลบริเวณ อ.เกาะยาว จ.พังงา</t>
-  </si>
-  <si>
     <t xml:space="preserve">7.85N , 98.54E </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบริเวณ จ. พังงา จ.ภูเก็ต และ จ.กระบี่</t>
-  </si>
-  <si>
     <t>7 พฤษภาคม 2558</t>
   </si>
   <si>
     <t>00:30</t>
   </si>
   <si>
-    <t>ใน ทะเลบริเวณ อ.เกาะยาว จ.พังงา</t>
-  </si>
-  <si>
     <t>7.84N , 98.51E</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวบริเวณ จ.พังงา จ.ภูเก็ต และ จ.กระบี</t>
-  </si>
-  <si>
     <t>24 พฤษภาคม 2558</t>
   </si>
   <si>
@@ -1453,51 +1195,21 @@
     <t>20.56N , 99.02E</t>
   </si>
   <si>
-    <t>รูสึกสั่นไหวบริเวณ จ.เชียงใหม จ.เชียงราย และ จ.แมฮองสอน</t>
-  </si>
-  <si>
     <t>14 กรกฎาคม 2558</t>
   </si>
   <si>
     <t>21:25</t>
   </si>
   <si>
-    <t>ต.ปรังเผล อ.สังขละบุรี จ.กาญจนบุรี</t>
-  </si>
-  <si>
-    <t>รูสึกสั่นไหวบริเวณ อ.สังขละบุรี, อ.ทองผาภูมิ จ.กาญจนบุรี</t>
-  </si>
-  <si>
     <t xml:space="preserve">San Sai, Chiang Mai </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนที่ San Sai, Chiang Mai</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mae Suai, Chiang Rai </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนที่ Mae Suai, Chiang Rai</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ Mae Suai, Chiang Rai</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mueang Chiang Rai, Chiang Rai </t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนที่ Mueang Chiang Rai, Chiang Rai</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.พาน,Mueang Chiang Rai, Chiang Rai</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นไหวบริเวณ Mueang Chiang Rai, Chiang Rai</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นไหว ที่บ้านและบนอาคาร อ.แม่สาย Mueang Chiang Rai, Chiang Rai</t>
-  </si>
-  <si>
     <t xml:space="preserve">Samoeng, Chiang Mai </t>
   </si>
   <si>
@@ -1540,33 +1252,15 @@
     <t xml:space="preserve">Phan, Chiang Rai </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ Phan, Chiang Rai กระจกและบ้านสั่น</t>
-  </si>
-  <si>
     <t>Mae Rim , Chiang Mai</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ Mae Rim , Chiang Maiและ จ.ลำพูน</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ Mae Rim , Chiang Mai</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ อ.เมือง Mae Rim , Chiang Mai</t>
-  </si>
-  <si>
-    <t>รู้สึกสั่นไหวได้ที่ Mae Rim , Chiang Mai</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mueang Mae Hong Son, Mae Hong Son  </t>
   </si>
   <si>
     <t>Wiang Pa Pao, Chiang Rai</t>
   </si>
   <si>
-    <t>รู้สึกสั่นสะเทือนได้ที่ Wiang Pa Pao, Chiang Raiและ จ. พะเยา</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Sumatra, Indonesia</t>
   </si>
   <si>
@@ -1597,9 +1291,6 @@
     <t xml:space="preserve">Phrasaeng, Surat Thani </t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวในบริเวณ Phrasaeng, Surat Thani</t>
-  </si>
-  <si>
     <t>Wiang Chai, Chiang Rai</t>
   </si>
   <si>
@@ -1621,9 +1312,6 @@
     <t>Mae Wang, Chiang Mai</t>
   </si>
   <si>
-    <t xml:space="preserve">รู้สึกสั่นสะเทือนได้ที่ อ.จอมทอง อ.เมือง Mae Wang, Chiang Mai </t>
-  </si>
-  <si>
     <t>Mueang Lampang, Lampang</t>
   </si>
   <si>
@@ -1633,29 +1321,299 @@
     <t>Mae Chan, Chiang Rai</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ ต.สันทราย Phrao, Chiang Mai</t>
-  </si>
-  <si>
     <t>Na Noi, Nan</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ Dok Khamtai, Phayao</t>
-  </si>
-  <si>
     <t>Dok Khamtai, Phayao</t>
   </si>
   <si>
-    <t>รู้สึกสั่นไหวที่ Thoen, Lampang</t>
-  </si>
-  <si>
     <t>Thoen, Lampang</t>
+  </si>
+  <si>
+    <t>Ko Yao, Phangnga</t>
+  </si>
+  <si>
+    <t>Sangkhla Buri, Kanchanaburi</t>
+  </si>
+  <si>
+    <t>Phuket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laos </t>
+  </si>
+  <si>
+    <t>Chiang Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiang Mai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chiang Rai </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at San Sai, Doi Saket, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Suai, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mueang Chiang Rai, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at San Sai, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mueang Chiang Mai, Hang Dong, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Rim , Chiang Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at Phuket </t>
+  </si>
+  <si>
+    <t>Seismic sensibility on high-rise buildings in Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phuket</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on high-rise buildings at Phuket</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at the northern part--Lampang, Chiang Mai, Chiang Rai and also at Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mueang Phuket, Phuket</t>
+  </si>
+  <si>
+    <t>Seismic sensibility away from Phuket to the southwest around 670 kilometers</t>
+  </si>
+  <si>
+    <t>Ther was no report of seismic sensibility in Thailand.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at the southern part and on the high-rise buildings in Bangkok.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility nearby epicenter.</t>
+  </si>
+  <si>
+    <t>Away from Chiang Mai to south around 110 km.</t>
+  </si>
+  <si>
+    <t>Away from Phuket to southwest around 700 km.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Away from Phuket to southwest around 640 km. </t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buildings in Chiang Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility on the high-rise buldings Chiang Mai and Lamphun </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Meaung Chiang Rai,  Thoeng, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Pa Daet, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Mai, Chiang Rai, Ma Hong Son</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at Chom Thong, Mueang Chiang Mai, Mae Wang, Chiang Mai </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at  Hang Dong, San Pa Tong, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Dao, Chiang Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at Prachuap Khiri Khan </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Prachuap Khiri Khan, Tha Yang, Phetchaburi, and Photharam, Ratchaburi, and Mueang Samut Songkhram, Samut Songkhram</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phan, Mueang Chiang Rai, Chiang Rai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at Hat Yai, Songkhla and Narathiwat </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Rim , Chiang Maiand Lamphun</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Mai and the high-rise buldings in Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Ma Hong Son</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Meaung Chiang Mai, Mae Rim , Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Wiang Pa Pao, Chiang Raiand, Phayao</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Rai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at the northern part and the high-rise buldingsin Bangkok </t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buldings in Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Saen, Chiang Rai andthe high-rise buldings in Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phangnga and Phuket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility on the high-rise buldings Phuket, Phangnga </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at almost province in the southern part, also the high-rise buildings in Bangkok and tsunami damage west of the southern part. Ther was almost 5,000 people killed by tsunami.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buildingsin Bangkok. There was almost 2,000 people died in China.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibilityat  Mae Rim, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phrasaeng, Surat Thani</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buildings in Bangkok.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buildingsin Bangkok.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buildings in Bangkok and Phuket. There was miniature tsunami nearby epicenter.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buildingsin Bangkok. Ther was alost 1,00 people died in Indonesia.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buldings in Phuket, Phannga, Surat Thani, Songkhla and Bangkok.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Sai, Mae Chan, Chiang Saen, Mae Fa Luang in Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phrae, Nan, Udon Thani, Loei, Nong Khai, Nong Bua Lam Phu, Khon Kaen, Mara Sarakham</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at the northern part , the northeast part and on the high-rise buildings in Bangkok. Also damaged at Mae Sai, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Sai, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Kantang, Yan Ta Khao, Mueang Trang in Trang</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mueang Phuket, Phuket and Hat Yai, Songkhla</t>
+  </si>
+  <si>
+    <t>Seismic sensibility nearby the epicenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at the southern part, the central region, also at the northeast part. Ther was tsunami 80 cm. in Indonesia and 30cm. at Meang island, Phangnga </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phuket. There was more than 26 aftershocks at Thalang, Phuket.</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mueang Ranong, Ranong</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on the high-rise buldings in Phuket and Songkhla</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phan, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Mai, Nonthaburi and Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Mai and on the high-rise buildings in Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility atMae Sai, Chiang Rai and on the high-rise buldings in Chiang Mai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at Lampang </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seismic sensibility at Mae Wang, Hang Dong, Meaung Chiang Mai in Chiang Mai </t>
+  </si>
+  <si>
+    <t>Seismic sensibility at the buidings in Mae Sai, Mueang Chiang Rai, Chiang Rai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Wang  San Pa Tong, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phuket, Phangnga and the high-rise buldings in Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Mae Chai, Phayao</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phrao, Chiang Mai</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Dok Khamtai, Phayao</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Meaung Phuket, Phuket</t>
+  </si>
+  <si>
+    <t>Seismic sensibility atChiang Rai, Phrae, Ma Hong Son, Uttaradit, Phitsanulok, Chiang Mai and the high-rise buildings in Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Meaung Nan, Nan</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Thoen, Lampang</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phangnga, Phuket and Krabi</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Chiang Mai, Chiang Rai and Mae Hong Son</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Sangkhla Buri, Thong Pha Phum, Kanchanaburi</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at the high-rise buildings in Chiang Rai, Chiang Mai and Bangkok</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Phangngaand Phuket</t>
+  </si>
+  <si>
+    <t>Seismic sensibility at Meaung Phuket, Kathu, Thalang in Phuket, Yao Yai island in Phangnga</t>
+  </si>
+  <si>
+    <t>Seismic sensibility on high-rise buildings in Mueang Chiang Mai, Chiang Mai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1664,6 +1622,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1686,9 +1649,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1992,8 +1956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2035,7 +1999,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>484</v>
+        <v>395</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -2043,1639 +2007,1639 @@
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
+      <c r="F2" s="2" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>487</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>490</v>
+      <c r="F4" s="2" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>485</v>
+        <v>448</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>27</v>
+      <c r="F6" s="2" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>37</v>
+        <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>455</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>495</v>
+        <v>399</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>500</v>
+        <v>404</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>58</v>
+        <v>454</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>68</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>77</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>501</v>
+        <v>405</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>502</v>
+        <v>406</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>91</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>96</v>
+        <v>462</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>500</v>
+        <v>404</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>101</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>106</v>
+        <v>485</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>504</v>
+        <v>408</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>111</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>106</v>
+        <v>528</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>119</v>
+        <v>485</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>122</v>
+        <v>443</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>125</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>128</v>
+        <v>444</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>488</v>
+        <v>446</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>128</v>
+        <v>444</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>134</v>
+        <v>466</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>128</v>
+        <v>444</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>139</v>
+        <v>467</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>505</v>
+        <v>409</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>468</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>147</v>
+        <v>442</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>535</v>
+        <v>469</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>506</v>
+        <v>410</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>152</v>
+        <v>470</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>506</v>
+        <v>410</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>157</v>
+        <v>471</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>162</v>
+        <v>472</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>162</v>
+        <v>472</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>162</v>
+        <v>472</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>498</v>
+        <v>402</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>174</v>
+        <v>473</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>507</v>
+        <v>411</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>182</v>
+        <v>475</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>187</v>
+        <v>477</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>511</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>195</v>
+        <v>162</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>511</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>514</v>
+        <v>413</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>198</v>
+        <v>165</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>199</v>
+        <v>478</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>511</v>
+        <v>450</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>512</v>
+        <v>479</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>515</v>
+        <v>414</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>516</v>
+        <v>480</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>215</v>
+        <v>451</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>216</v>
+        <v>181</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>217</v>
+        <v>182</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>518</v>
+        <v>416</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>218</v>
+        <v>183</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>219</v>
+        <v>481</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>519</v>
+        <v>417</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>223</v>
+        <v>482</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>510</v>
+        <v>476</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>230</v>
+        <v>402</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>233</v>
+        <v>484</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>238</v>
+        <v>483</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>242</v>
+        <v>202</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>243</v>
+        <v>483</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>244</v>
+        <v>203</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>245</v>
+        <v>204</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>521</v>
+        <v>419</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>246</v>
+        <v>205</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>219</v>
+        <v>481</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>247</v>
+        <v>206</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>248</v>
+        <v>207</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>520</v>
+        <v>418</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>249</v>
+        <v>208</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>219</v>
+        <v>481</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>252</v>
+        <v>211</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>517</v>
+        <v>415</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>253</v>
+        <v>212</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>254</v>
+        <v>486</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>257</v>
+        <v>215</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>258</v>
+        <v>216</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>259</v>
+        <v>494</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>261</v>
+        <v>218</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>509</v>
+        <v>412</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>262</v>
+        <v>219</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>513</v>
+        <v>490</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>522</v>
+        <v>420</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>265</v>
+        <v>222</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>267</v>
+        <v>488</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>523</v>
+        <v>421</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>270</v>
+        <v>226</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>271</v>
+        <v>227</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>272</v>
+        <v>489</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>524</v>
+        <v>422</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>276</v>
+        <v>493</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>277</v>
+        <v>231</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>278</v>
+        <v>232</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>525</v>
+        <v>423</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>279</v>
+        <v>233</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>280</v>
+        <v>234</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>281</v>
+        <v>492</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>282</v>
+        <v>235</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>283</v>
+        <v>236</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>526</v>
+        <v>424</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>284</v>
+        <v>237</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>527</v>
+        <v>491</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>285</v>
+        <v>238</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>286</v>
+        <v>239</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>287</v>
+        <v>240</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>288</v>
+        <v>241</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>289</v>
+        <v>495</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>219</v>
+        <v>481</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>528</v>
+        <v>425</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>492</v>
+        <v>447</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>302</v>
+        <v>483</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>303</v>
+        <v>254</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>304</v>
+        <v>255</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>305</v>
+        <v>256</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>306</v>
+        <v>257</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>307</v>
+        <v>496</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>230</v>
+        <v>402</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>311</v>
+        <v>497</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>312</v>
+        <v>261</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>313</v>
+        <v>262</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>503</v>
+        <v>407</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>314</v>
+        <v>263</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>315</v>
+        <v>483</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>316</v>
+        <v>264</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>317</v>
+        <v>265</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>318</v>
+        <v>441</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>319</v>
+        <v>266</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>321</v>
+        <v>498</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>322</v>
+        <v>268</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>323</v>
+        <v>269</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>230</v>
+        <v>402</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>324</v>
+        <v>270</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>325</v>
+        <v>271</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>326</v>
+        <v>499</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>327</v>
+        <v>272</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>328</v>
+        <v>273</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>495</v>
+        <v>399</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>329</v>
+        <v>274</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>330</v>
+        <v>453</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>331</v>
+        <v>275</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>332</v>
+        <v>276</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>230</v>
+        <v>402</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>333</v>
+        <v>277</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>334</v>
+        <v>278</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>335</v>
+        <v>500</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>336</v>
+        <v>279</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>337</v>
+        <v>280</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>529</v>
+        <v>426</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>338</v>
+        <v>281</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>339</v>
+        <v>501</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>340</v>
+        <v>282</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>341</v>
+        <v>283</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>342</v>
+        <v>284</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>325</v>
+        <v>271</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>343</v>
+        <v>502</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>344</v>
+        <v>285</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>345</v>
+        <v>286</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>530</v>
+        <v>427</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>346</v>
+        <v>287</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>347</v>
+        <v>288</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>348</v>
+        <v>503</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>349</v>
+        <v>289</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>350</v>
+        <v>290</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>496</v>
+        <v>400</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>351</v>
+        <v>291</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>280</v>
+        <v>234</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>352</v>
+        <v>453</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>353</v>
+        <v>292</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>354</v>
+        <v>293</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>355</v>
+        <v>294</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>357</v>
+        <v>504</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>358</v>
+        <v>296</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>359</v>
+        <v>297</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>531</v>
+        <v>428</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>360</v>
+        <v>298</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>361</v>
+        <v>299</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>362</v>
+        <v>505</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>363</v>
+        <v>300</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>364</v>
+        <v>301</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>532</v>
+        <v>429</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>365</v>
+        <v>302</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>334</v>
+        <v>278</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>366</v>
+        <v>506</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>367</v>
+        <v>303</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>368</v>
+        <v>304</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>369</v>
+        <v>305</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>370</v>
+        <v>306</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>371</v>
+        <v>507</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>372</v>
+        <v>307</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>373</v>
+        <v>308</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>533</v>
+        <v>430</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>374</v>
+        <v>309</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>508</v>
@@ -3683,522 +3647,522 @@
     </row>
     <row r="85" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>375</v>
+        <v>310</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>376</v>
+        <v>311</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>377</v>
+        <v>312</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>378</v>
+        <v>313</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>379</v>
+        <v>509</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>375</v>
+        <v>310</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>380</v>
+        <v>314</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>381</v>
+        <v>315</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>382</v>
+        <v>510</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>383</v>
+        <v>316</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>384</v>
+        <v>317</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>385</v>
+        <v>318</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>386</v>
+        <v>319</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>387</v>
+        <v>511</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>388</v>
+        <v>320</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>389</v>
+        <v>321</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>390</v>
+        <v>322</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>361</v>
+        <v>299</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>391</v>
+        <v>500</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>392</v>
+        <v>323</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>393</v>
+        <v>324</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>536</v>
+        <v>432</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>394</v>
+        <v>325</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>395</v>
+        <v>512</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>396</v>
+        <v>326</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>397</v>
+        <v>327</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>534</v>
+        <v>431</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>398</v>
+        <v>328</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>399</v>
+        <v>329</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>400</v>
+        <v>513</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>401</v>
+        <v>330</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>402</v>
+        <v>331</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>403</v>
+        <v>332</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>404</v>
+        <v>478</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>405</v>
+        <v>333</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>406</v>
+        <v>334</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>407</v>
+        <v>335</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>320</v>
+        <v>267</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>493</v>
+        <v>514</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>408</v>
+        <v>336</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>409</v>
+        <v>337</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>534</v>
+        <v>431</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>410</v>
+        <v>338</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>411</v>
+        <v>515</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>412</v>
+        <v>339</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>413</v>
+        <v>340</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>497</v>
+        <v>401</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>414</v>
+        <v>341</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>415</v>
+        <v>342</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>416</v>
+        <v>516</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>417</v>
+        <v>343</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>418</v>
+        <v>344</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>537</v>
+        <v>433</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>419</v>
+        <v>345</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>420</v>
+        <v>346</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>421</v>
+        <v>517</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>422</v>
+        <v>347</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>423</v>
+        <v>348</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>538</v>
+        <v>434</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>425</v>
+        <v>350</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>391</v>
+        <v>500</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>426</v>
+        <v>351</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>427</v>
+        <v>352</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>523</v>
+        <v>421</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>428</v>
+        <v>353</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>539</v>
+        <v>518</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>429</v>
+        <v>354</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>430</v>
+        <v>355</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>537</v>
+        <v>433</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>431</v>
+        <v>356</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>432</v>
+        <v>357</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>433</v>
+        <v>358</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>434</v>
+        <v>359</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>500</v>
+        <v>404</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>435</v>
+        <v>360</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>436</v>
+        <v>361</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>437</v>
+        <v>520</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>438</v>
+        <v>362</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>439</v>
+        <v>363</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>533</v>
+        <v>430</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>440</v>
+        <v>364</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>370</v>
+        <v>306</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>441</v>
+        <v>521</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>442</v>
+        <v>365</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>389</v>
+        <v>321</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>540</v>
+        <v>435</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>443</v>
+        <v>366</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>444</v>
+        <v>522</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>445</v>
+        <v>367</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>446</v>
+        <v>368</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>542</v>
+        <v>436</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>447</v>
+        <v>369</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>541</v>
+        <v>519</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>448</v>
+        <v>370</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>449</v>
+        <v>371</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>450</v>
+        <v>372</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>451</v>
+        <v>373</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>452</v>
+        <v>374</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>453</v>
+        <v>527</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>454</v>
+        <v>375</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>544</v>
+        <v>437</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>456</v>
+        <v>377</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>543</v>
+        <v>523</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>457</v>
+        <v>378</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>458</v>
+        <v>379</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>460</v>
+        <v>380</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>334</v>
+        <v>278</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>461</v>
+        <v>529</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>462</v>
+        <v>381</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>463</v>
+        <v>382</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>465</v>
+        <v>383</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>271</v>
+        <v>227</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>461</v>
+        <v>529</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>466</v>
+        <v>384</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>467</v>
+        <v>385</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>468</v>
+        <v>438</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>469</v>
+        <v>386</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>386</v>
+        <v>319</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>470</v>
+        <v>524</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>471</v>
+        <v>387</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>472</v>
+        <v>388</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>473</v>
+        <v>438</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>474</v>
+        <v>389</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>475</v>
+        <v>524</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>476</v>
+        <v>390</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>477</v>
+        <v>391</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>499</v>
+        <v>403</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>478</v>
+        <v>392</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>479</v>
+        <v>525</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>480</v>
+        <v>393</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>481</v>
+        <v>394</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>482</v>
+        <v>439</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>478</v>
+        <v>392</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>483</v>
+        <v>526</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11323,5 +11287,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>